<commit_message>
SWBM files updated through wy2018, but SWBM is not running for new model period
email to gus: I've updated the following input files:
kc_alfalfa.txt
kc_pasture.txt
kc_grain.txt
precip.txt
ref_et.txt
streamflow_input.txt (ran a new regression)

I've also changed the number of stress periods in the general_inputs.txt. (It's now 336.)

I can't find any obvious changes I need to make in the SWBM.f90 file. It looks like it should iterate over nmonths, which it reads out of general_inputs.txt. Am I missing any files/parameters that I need to update?
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7059C14-352E-44CE-92FA-F5596587026E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4CBCDE-C97B-4F76-B9F6-2307D1603B4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stress_period_table" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
   <si>
     <t>year</t>
   </si>
@@ -344,6 +344,33 @@
   </si>
   <si>
     <t>14/07/2011</t>
+  </si>
+  <si>
+    <t>kc_pasture.txt</t>
+  </si>
+  <si>
+    <t>kc_grain.txt</t>
+  </si>
+  <si>
+    <t>extended table. Replicated kc curve. Start dates always 3/10 now.</t>
+  </si>
+  <si>
+    <t>ref_et.txt</t>
+  </si>
+  <si>
+    <t>Downloaded daily Eto from Cimis in Scott. Added daily data on to existing ET record (new data starting 2011)</t>
+  </si>
+  <si>
+    <t>streamflow_input.txt</t>
+  </si>
+  <si>
+    <t>Downloaded fort jones stream gauge info from USGS. Added daily data onto existing stream record and re-regressed to get tributary flows for 2011-2018.</t>
+  </si>
+  <si>
+    <t>precip.txt</t>
+  </si>
+  <si>
+    <t>Downloaded daily precip from NOAA. Added daily data on to existing ET record (new data starting 2011)</t>
   </si>
 </sst>
 </file>
@@ -701,7 +728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F339"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A309" workbookViewId="0">
+      <selection activeCell="B337" sqref="B337"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9087,16 +9116,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292E7DA5-4614-486F-98A1-92BE8CF4B7A6}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -9138,6 +9167,61 @@
       </c>
       <c r="C3" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -9150,7 +9234,7 @@
   <dimension ref="A1:G2610"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32402,8 +32486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E804045-79F7-4E7D-8B19-2A8DBB89F569}">
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D128" sqref="D1:D128"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
SWBM now working but throws an error on final month. updated DIS file for modflow run
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4CBCDE-C97B-4F76-B9F6-2307D1603B4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D921AB7-CFD5-44EE-8003-D9A0F62EA127}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
   <si>
     <t>year</t>
   </si>
@@ -371,6 +371,33 @@
   </si>
   <si>
     <t>Downloaded daily precip from NOAA. Added daily data on to existing ET record (new data starting 2011)</t>
+  </si>
+  <si>
+    <t>Drains_initial_m3day.txt</t>
+  </si>
+  <si>
+    <t>was 252 zeros; now 336 zeros</t>
+  </si>
+  <si>
+    <t>Drains_m3day.txt</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">252 &gt; 336 stress periods at top. Added 7 years of Data Set 7 (period length (days/months)). </t>
+  </si>
+  <si>
+    <t>Is the big bulk of this file Dataset 5?</t>
+  </si>
+  <si>
+    <t>hob</t>
+  </si>
+  <si>
+    <t>other modflow files??</t>
+  </si>
+  <si>
+    <t>fix the swbm outputttt</t>
   </si>
 </sst>
 </file>
@@ -9116,10 +9143,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292E7DA5-4614-486F-98A1-92BE8CF4B7A6}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9222,6 +9249,54 @@
       </c>
       <c r="C8" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ck gets familiar with the .wel package
comment out pval filename in .nam (fixed "PARAMETER "DRN_5000 " IN PARAMETER INPUT FILE HAS NOT BEEN DEFINED" error)

At to do list items to notes.xlsx. put in placeholders for to do list items in Generate_SWBM_Inputs.R.
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F438D9F9-0B79-4D57-8025-57A35FEE86ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3740AE3A-800B-45F6-ACDA-5CA5E5D57713}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2892" yWindow="0" windowWidth="19476" windowHeight="12372" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stress_period_table" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="143">
   <si>
     <t>year</t>
   </si>
@@ -412,9 +412,6 @@
     <t>extended table of 10000 drain conductance for each discharge zone cell</t>
   </si>
   <si>
-    <t>Update SWBM production of Well file. Change "wel5" to "mfr" variable names; reduce text redundancy</t>
-  </si>
-  <si>
     <t>to do^</t>
   </si>
   <si>
@@ -422,6 +419,45 @@
   </si>
   <si>
     <t>update wl obs</t>
+  </si>
+  <si>
+    <t>"parameter" wells and "nonparameter" wells. Wtf?</t>
+  </si>
+  <si>
+    <t>wel package decoding. Section: "wel5 Q ## #### INSTANCES". "Stress1".</t>
+  </si>
+  <si>
+    <t>Each row under stress1 is a cell in the MFR. YOU SHOULD RENAME THESE TO BE MFR.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section just turns MFR on and off for different months. It's so fcking redundant. </t>
+  </si>
+  <si>
+    <t>wel package decoding. Section: "### 9 Stress Period 1".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then each of the MFR recharge cells are invoked below it. </t>
+  </si>
+  <si>
+    <t>Each row here is for the pumping numbers for an actual well. Calculated from SWBM.</t>
+  </si>
+  <si>
+    <t>TO DO: ADD "Stress253-Stress336" to each mfr.</t>
+  </si>
+  <si>
+    <t>Change the names to reference MFRs and ditches.</t>
+  </si>
+  <si>
+    <t>TO DO: Tab files?</t>
+  </si>
+  <si>
+    <t>change param names to MFRs.</t>
+  </si>
+  <si>
+    <t>Confirm I don't need a Stress 336.</t>
+  </si>
+  <si>
+    <t>to do: Change "instance" from 252 to 336. Only goes through 335 - need a 336 stress?</t>
   </si>
 </sst>
 </file>
@@ -11889,10 +11925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292E7DA5-4614-486F-98A1-92BE8CF4B7A6}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12062,21 +12098,82 @@
       <c r="B14" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>127</v>
+      <c r="C14" s="11"/>
+      <c r="D14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
in middle of new Input Generation reorganization
steps:
- new folder structure to hold input files that don't change with updated model period, and store new input files for things like changing precip scenarios
- new inventory in notes.xlsx for tracking input file tasks. Going to turn this into an input file dictionary.
- Generate_SVIHM_Inputs.R reorganized (very in progress)
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3740AE3A-800B-45F6-ACDA-5CA5E5D57713}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA47C54-A321-4326-8550-7DA6AB3FF54F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2892" yWindow="0" windowWidth="19476" windowHeight="12372" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19950" yWindow="-4680" windowWidth="18780" windowHeight="8970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stress_period_table" sheetId="1" r:id="rId1"/>
     <sheet name="input_file_changes" sheetId="2" r:id="rId2"/>
-    <sheet name="scratch work" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="input_file_dictionary" sheetId="5" r:id="rId3"/>
+    <sheet name="scratch work" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">input_file_dictionary!$B$6:$E$31</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="205">
   <si>
     <t>year</t>
   </si>
@@ -421,9 +425,6 @@
     <t>update wl obs</t>
   </si>
   <si>
-    <t>"parameter" wells and "nonparameter" wells. Wtf?</t>
-  </si>
-  <si>
     <t>wel package decoding. Section: "wel5 Q ## #### INSTANCES". "Stress1".</t>
   </si>
   <si>
@@ -445,19 +446,208 @@
     <t>TO DO: ADD "Stress253-Stress336" to each mfr.</t>
   </si>
   <si>
-    <t>Change the names to reference MFRs and ditches.</t>
-  </si>
-  <si>
     <t>TO DO: Tab files?</t>
-  </si>
-  <si>
-    <t>change param names to MFRs.</t>
   </si>
   <si>
     <t>Confirm I don't need a Stress 336.</t>
   </si>
   <si>
     <t>to do: Change "instance" from 252 to 336. Only goes through 335 - need a 336 stress?</t>
+  </si>
+  <si>
+    <t>"parameter" wells and "nonparameter" wells. "Parameter" wells are ones that can be adjusted during calibration. Nonparameter wells are specified. In this case, the parameter wells are the Mountain Front Recharge (MFR) locations and the leaking ditches (Farmer's and SVID).</t>
+  </si>
+  <si>
+    <t>Change the names to reference MFRs and ditches. Have to do this in the SWBM source script (and the template file), since that's where .WEL gets written. Gus has done this. Thanks Gus.</t>
+  </si>
+  <si>
+    <t>change param names to MFRs. Gus has done this. Thanks Gus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEXT TO DO ITEM: Make the generator script create the .DRN file. Use Gus' script. </t>
+  </si>
+  <si>
+    <t>crop_coeff_mult.txt</t>
+  </si>
+  <si>
+    <t>daily_out.txt</t>
+  </si>
+  <si>
+    <t>ET_Cells_DZ.txt</t>
+  </si>
+  <si>
+    <t>irr_eff.txt</t>
+  </si>
+  <si>
+    <t>MAR_Fields.txt</t>
+  </si>
+  <si>
+    <t>No_Flow_SVIHM.txt</t>
+  </si>
+  <si>
+    <t>polygons_table.txt</t>
+  </si>
+  <si>
+    <t>Recharge_Zones_SVIHM.txt</t>
+  </si>
+  <si>
+    <t>SFR_PEST_TPL.txt</t>
+  </si>
+  <si>
+    <t>SFR_UCODE_JTF.txt</t>
+  </si>
+  <si>
+    <t>SVIHM_ETS_template.txt</t>
+  </si>
+  <si>
+    <t>SVIHM_SFR_template.txt</t>
+  </si>
+  <si>
+    <t>SVIHM_WEL_template.txt</t>
+  </si>
+  <si>
+    <t>well_list_by_polygon.txt</t>
+  </si>
+  <si>
+    <t>well_summary.txt</t>
+  </si>
+  <si>
+    <t>Input File Name</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>SWBM</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>??? How different from the kc_alfalfa.txt files?</t>
+  </si>
+  <si>
+    <t>For each polygon in this list, SWBM writes a text file with the budget for that field. (??) Contains a list of fields in different categories defined by crop type, irrigation source, and irrigation tech. Also some misc fields associated with MAR and some mystery ones on the end.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of 0s, one flow for each stress period. Used to represent initial flow in drains. </t>
+  </si>
+  <si>
+    <t>Starts as a list of 0s, one for each stress period. Gets written over in the .bat script?</t>
+  </si>
+  <si>
+    <t>Grid of 0s and 1s. Cells with 1s are cells in the model grid within the Discharge Zone.</t>
+  </si>
+  <si>
+    <t>Questions?</t>
+  </si>
+  <si>
+    <t>Number of: fields, irrigation wells, stress periods, rows, and columns. RD_Mult? Also specifies UCODE or PEST calibration, and which scenario is running.</t>
+  </si>
+  <si>
+    <t>Effective irrigation efficiencies for flood; for alfalfa-wheel line and alfalfa-center pivot; and for pasture-wheel line and pasture-center pivot.</t>
+  </si>
+  <si>
+    <t>Time-dependent crop coefficient, Kc, for alfalfa. Day by day for whole model period. "Growing season" value of 0.9 for Mar 1-Oct 30; "dormant" value of 0 for Nov 1-Feb28/29.</t>
+  </si>
+  <si>
+    <t>Time-dependent crop coefficient, Kc, for pasture. Day by day for whole model period. "Growing season" value of 0.9 for Mar 1-Oct 30; "dormant" value of 0 for Nov 1-Feb28/29.</t>
+  </si>
+  <si>
+    <t>Why are growing season start dates different year to year? Kc curve for the growing season. See generate_inputs script for equation used to generate curve.</t>
+  </si>
+  <si>
+    <t>List of fields used in MAR scenario, and assumed  maximum infiltration rate (into soil column or deeper aquifer?)</t>
+  </si>
+  <si>
+    <t>Grid of 0s and 1s. Cells with 0 are no-flow.</t>
+  </si>
+  <si>
+    <t>Table listing fields/parcels/polygons within the model domain, and associated land use and other properties.</t>
+  </si>
+  <si>
+    <t>Daily precip for whole model period, in meters.</t>
+  </si>
+  <si>
+    <t>???? Field IDs?</t>
+  </si>
+  <si>
+    <t>Daily reference ET in meters and then in inches. Why did we choose to have consistent monthly ET values? Should I preserve those during the model update, or use daily values? Should I use daily values going forward?</t>
+  </si>
+  <si>
+    <t>Key:</t>
+  </si>
+  <si>
+    <t>I should know this</t>
+  </si>
+  <si>
+    <t>This is critical to updating the model</t>
+  </si>
+  <si>
+    <t>Cannot proceed without this information</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I will need to know this for calibration, or This is really bugging me</t>
+  </si>
+  <si>
+    <t>Monthly streamflow, in monthly average flowrate (cubic meters per day). Generated using Streamflow Regression R script.</t>
+  </si>
+  <si>
+    <t>SFR calibration template file. What do these columns mean? Ptf?</t>
+  </si>
+  <si>
+    <t>ETS input template. ETS used to simulate ET from the saturated zone. We have no parameters because we don't calibrate on ET? (but don't we? We calibrate using the kc values.) Do we not have a Data Set 2? In Data Set 4, what does INETSS mean? What are all these numbers? Starting points for ET?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why is thickness and conductivity always 1 and 10? SFR input template. Stream-Flow Routing. Each row pertains to a "reach." Reaches belong to longer "segments." Each row contains the following info: layer, row, column, segment, reach number. Reach length, elevation, slope. Streambed thickness and conductivity (1 and 10). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEL input template. Defines 9 parameters (MFR5-11, FRMRSDitch, SVIDDitch). The definition consists of listing the layer, row, column and flowrate of each cell associated with that mountain front recharge section or the two ditches. Water flow into those cells is uniform across each of the defined sections/ditches. I believe these were defined to match the older SV model from S. S. Papadopulous. Each parameter has a flowrate multiplier specified at the top, which applies to each cell in the definition, and can be altered during calibration. How did we/Papadopulous find these MFR and Ditch infiltration numbers? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log number (associated with Well Completion Reports), layer the well pulls from, row, column, easting and northing. </t>
+  </si>
+  <si>
+    <t>Streamflow regression</t>
+  </si>
+  <si>
+    <t>File generation scripted?</t>
+  </si>
+  <si>
+    <t>A lookup table associating polygons (fields) with (the closest?) well used to irrigate it. Assigns irrigation demanded by ET on that field to a specific well (which is then applied to a specific cell). Method for associating field with a well?</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>To do: combine streamflow inputs into one file. Make this a function callable from Generate_Inputs.</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>draft</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>draft, final tbd</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>don't need to at this time</t>
+  </si>
+  <si>
+    <t>MODFLOW</t>
   </si>
 </sst>
 </file>
@@ -484,7 +674,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +684,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -561,6 +781,52 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11925,10 +12191,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292E7DA5-4614-486F-98A1-92BE8CF4B7A6}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12100,7 +12366,7 @@
       </c>
       <c r="C14" s="11"/>
       <c r="D14" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -12118,62 +12384,67 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
-        <v>138</v>
+      <c r="B21" s="12" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
-        <v>140</v>
+      <c r="B26" s="12" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B28" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -12182,6 +12453,464 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="76.77734375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" s="25"/>
+      <c r="E25" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D29" s="27"/>
+      <c r="E29" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="33" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45834955-FDB1-49F5-8590-B53D8262CCAA}">
   <dimension ref="A1:G2610"/>
   <sheetViews>
@@ -35434,12 +36163,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E804045-79F7-4E7D-8B19-2A8DBB89F569}">
   <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Script the update for SVIHM.dis file
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8848AA73-73EB-418F-BC78-700336DE8783}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E380899-A62B-44DD-A5EF-4F1AEEEC9606}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13440" yWindow="4800" windowWidth="9600" windowHeight="6528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_file_dictionary" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
   <si>
     <t>year</t>
   </si>
@@ -448,6 +448,35 @@
   </si>
   <si>
     <t>SWBM and Streamflow Regression</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Indicates cells that are active in the model using 1s (active) and 0s (not active). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">25I3? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Calls the two text files containing the starting heads for Layer 1 and Layer 2. </t>
+    </r>
+  </si>
+  <si>
+    <t>Provides variables to define discretization in space and time, and units. Flag indicating no quasi-3D confining bed in either layer. Grid of numbers indicating the elevation (meters above mean sea level) of the top of the model domain; the bottom of layer 1; and the bottom of layer 2.</t>
   </si>
 </sst>
 </file>
@@ -571,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -638,6 +667,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,8 +1310,8 @@
       <c r="B26" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>114</v>
+      <c r="C26" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="20" t="s">
@@ -1295,8 +1325,8 @@
       <c r="B27" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>114</v>
+      <c r="C27" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="20" t="s">
@@ -1310,8 +1340,8 @@
       <c r="B28" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>114</v>
+      <c r="C28" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="20" t="s">
@@ -1361,31 +1391,35 @@
       <c r="D31" s="16"/>
       <c r="E31" s="30"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="30"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="32"/>
+      <c r="E32" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>114</v>
+      <c r="C33" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="D33" s="16"/>
-      <c r="E33" s="30"/>
+      <c r="E33" s="30" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">

</xml_diff>

<commit_message>
.hob file update script in progress.
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E380899-A62B-44DD-A5EF-4F1AEEEC9606}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8638446-7C01-4EA3-914F-7DEDF57D64C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="4800" windowWidth="9600" windowHeight="6528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_file_dictionary" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="148">
   <si>
     <t>year</t>
   </si>
@@ -478,6 +478,63 @@
   <si>
     <t>Provides variables to define discretization in space and time, and units. Flag indicating no quasi-3D confining bed in either layer. Grid of numbers indicating the elevation (meters above mean sea level) of the top of the model domain; the bottom of layer 1; and the bottom of layer 2.</t>
   </si>
+  <si>
+    <t>Defines the Discharge Zone (DZ) as a parameter. Each cell in the discharge zone is assigned an elevation and conductance. Then repeats the DZ parameter for each timestep.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Specifies gauge locations (stream segment and reach) and output format (units and output values. Currently set at 4, which includes time, stage, outflow, depth, width, flow at midpoint, streambed condunctance for reach, head difference across streambed, and hydraulic gradient across the streambed. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What are all these commented-out gages? Are those for other predictions?</t>
+    </r>
+  </si>
+  <si>
+    <t>SVIHM.sfr</t>
+  </si>
+  <si>
+    <t>Written by SWBM</t>
+  </si>
+  <si>
+    <t>SVIHM.ets</t>
+  </si>
+  <si>
+    <t>getting there</t>
+  </si>
+  <si>
+    <r>
+      <t>Head observation file. Preamble, then, for each well, a row containing: location name, layer, row, column, number of stress periods containing an observation (listed as a negative number), an offset time from the start of the stress period (seems to be used for a structure where each location has one obselvation; it's just 0 for all of ours), row and column offset from center of cell (as fractions of cell width or height; all of ours are located in the middle of a quadrant, specified with + or - 0.25 offsets), and some extra parameters. For each observation under that well, list the unique observation identifier (built on the location name), the stress period in which the measurement was made, the number of time steps into the stress period, the head measurement (meters above mean sea level), and some extra parameters.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> How do we connect the CASGEM ids with the DWR_2 ids in the model? Lat/long? What's the fastest way to add new wells to this file? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Make to do list in here</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -500,7 +557,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,12 +608,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -600,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -653,10 +704,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -666,7 +717,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -683,6 +733,804 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="$TOGGLE0186AC_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD60CF86-27C1-48C0-8E71-02982C5CA69E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="23225760"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="$TOGGLE0186AD_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1628DDC5-DF49-4791-8055-22949EE4CC95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="23591520"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="$TOGGLE0186AE_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9432E248-FAD8-4AD7-8687-154A7BCB342F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="23774400"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="$TOGGLE0186AF_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E51F9C44-066D-4C48-81DE-F0211C8B2A8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="23957280"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="$TOGGLE0186B0_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C0EE5F2-CEB1-435C-A40C-1D18538E675F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="24140160"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="$TOGGLE0186B1_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D5B1A2-7D6E-4CCA-A15D-355F5823144F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="24505920"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="$TOGGLE0186B2_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A139CE3-20E9-47CF-B733-FC25FED9C2E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="24688800"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="$TOGGLE0186B3_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AB1963E-F0CF-4501-86F5-4985EE0909E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="24871680"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="$TOGGLE0186B4_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00066523-322E-4FBC-BFE4-BC79C51EAB23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="25054560"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="$TOGGLE0186B5_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0EDEC47-DC6E-4284-850C-EE10A8ECCEA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="25237440"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="$TOGGLE0186B6_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A2BF008-EADD-4A5A-9638-CBA944A730D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="25420320"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="$TOGGLE0186B7_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E829F70-D041-4FE1-9F86-14A4C56C0192}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="25786080"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="$TOGGLE0186B8_ICON" descr="hmtoggle_plus1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C1DCF50-6ECA-49D0-AB8B-B41F3BE8BDEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2430780" y="25968960"/>
+          <a:ext cx="83820" cy="83820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -948,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1401,7 +2249,7 @@
       <c r="C32" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="30" t="s">
         <v>139</v>
       </c>
@@ -1421,64 +2269,72 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="31" t="s">
-        <v>117</v>
+      <c r="C34" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="D34" s="16"/>
-      <c r="E34" s="30"/>
+      <c r="E34" s="30" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>114</v>
+        <v>145</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D35" s="16"/>
-      <c r="E35" s="30"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="30"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="31"/>
+      <c r="E36" s="30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="30"/>
+        <v>146</v>
+      </c>
+      <c r="D37" s="31"/>
+      <c r="E37" s="30" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>114</v>
@@ -1491,7 +2347,7 @@
         <v>122</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>114</v>
@@ -1504,7 +2360,7 @@
         <v>122</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>114</v>
@@ -1517,7 +2373,7 @@
         <v>122</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>114</v>
@@ -1526,24 +2382,24 @@
       <c r="E41" s="30"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="28" t="s">
-        <v>122</v>
-      </c>
+      <c r="A42" s="28"/>
       <c r="B42" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>114</v>
+        <v>143</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D42" s="16"/>
-      <c r="E42" s="30"/>
+      <c r="E42" s="30" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>114</v>
@@ -1556,20 +2412,22 @@
         <v>122</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>114</v>
+        <v>47</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D44" s="16"/>
-      <c r="E44" s="30"/>
+      <c r="E44" s="30" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="28" t="s">
         <v>122</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>114</v>
@@ -1582,7 +2440,7 @@
         <v>122</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>114</v>
@@ -1590,9 +2448,109 @@
       <c r="D46" s="16"/>
       <c r="E46" s="30"/>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="30"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="16"/>
+      <c r="E48" s="30"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="30"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E75"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E76"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E77"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E78"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E79"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E80"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E81"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E82"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E83"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E84"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E85"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E86"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E87"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E88"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E89"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E90"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E91"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E92"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E93"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E94"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
.hob scripting in progress
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8638446-7C01-4EA3-914F-7DEDF57D64C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907A6F57-74E4-40E0-BFCD-34E301B6774D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_file_dictionary" sheetId="5" r:id="rId1"/>
@@ -651,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,6 +718,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1798,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -2558,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H339"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="H337" sqref="H337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2624,8 +2625,8 @@
         <v>33147</v>
       </c>
       <c r="H2" s="7">
-        <f>G2-DATE(1990, 9, 1)</f>
-        <v>30</v>
+        <f>G3-DATE(1990,10, 1)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2652,8 +2653,8 @@
         <v>33178</v>
       </c>
       <c r="H3">
-        <f>G3-G2</f>
-        <v>31</v>
+        <f>G4-G3</f>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2680,8 +2681,8 @@
         <v>33208</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H67" si="1">G4-G3</f>
-        <v>30</v>
+        <f t="shared" ref="H4:H67" si="1">G5-G4</f>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2737,7 +2738,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2765,7 +2766,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2793,7 +2794,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2821,7 +2822,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2849,7 +2850,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2877,7 +2878,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2933,7 +2934,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2966,7 +2967,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2999,7 +3000,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -3032,7 +3033,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -3098,7 +3099,7 @@
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -3131,7 +3132,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -3164,7 +3165,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -3197,7 +3198,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -3230,7 +3231,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -3263,7 +3264,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -3329,7 +3330,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -3362,7 +3363,7 @@
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -3395,7 +3396,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -3428,7 +3429,7 @@
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -3494,7 +3495,7 @@
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -3527,7 +3528,7 @@
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -3560,7 +3561,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -3593,7 +3594,7 @@
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -3626,7 +3627,7 @@
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -3659,7 +3660,7 @@
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -3725,7 +3726,7 @@
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3758,7 +3759,7 @@
       </c>
       <c r="H38">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -3791,7 +3792,7 @@
       </c>
       <c r="H39">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -3824,7 +3825,7 @@
       </c>
       <c r="H40">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -3890,7 +3891,7 @@
       </c>
       <c r="H42">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -3923,7 +3924,7 @@
       </c>
       <c r="H43">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -3956,7 +3957,7 @@
       </c>
       <c r="H44">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -3989,7 +3990,7 @@
       </c>
       <c r="H45">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -4022,7 +4023,7 @@
       </c>
       <c r="H46">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -4055,7 +4056,7 @@
       </c>
       <c r="H47">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -4121,7 +4122,7 @@
       </c>
       <c r="H49">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -4154,7 +4155,7 @@
       </c>
       <c r="H50">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -4187,7 +4188,7 @@
       </c>
       <c r="H51">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -4220,7 +4221,7 @@
       </c>
       <c r="H52">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -4286,7 +4287,7 @@
       </c>
       <c r="H54">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -4319,7 +4320,7 @@
       </c>
       <c r="H55">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -4352,7 +4353,7 @@
       </c>
       <c r="H56">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -4385,7 +4386,7 @@
       </c>
       <c r="H57">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -4418,7 +4419,7 @@
       </c>
       <c r="H58">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -4451,7 +4452,7 @@
       </c>
       <c r="H59">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -4517,7 +4518,7 @@
       </c>
       <c r="H61">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -4550,7 +4551,7 @@
       </c>
       <c r="H62">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -4583,7 +4584,7 @@
       </c>
       <c r="H63">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -4616,7 +4617,7 @@
       </c>
       <c r="H64">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -4682,7 +4683,7 @@
       </c>
       <c r="H66">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -4715,7 +4716,7 @@
       </c>
       <c r="H67">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -4747,8 +4748,8 @@
         <v>35156</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="H68:H131" si="60">G68-G67</f>
-        <v>31</v>
+        <f t="shared" ref="H68:H131" si="60">G69-G68</f>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -4781,7 +4782,7 @@
       </c>
       <c r="H69">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -4814,7 +4815,7 @@
       </c>
       <c r="H70">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -4847,7 +4848,7 @@
       </c>
       <c r="H71">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -4913,7 +4914,7 @@
       </c>
       <c r="H73">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -4946,7 +4947,7 @@
       </c>
       <c r="H74">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -4979,7 +4980,7 @@
       </c>
       <c r="H75">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
@@ -5012,7 +5013,7 @@
       </c>
       <c r="H76">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -5078,7 +5079,7 @@
       </c>
       <c r="H78">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
@@ -5111,7 +5112,7 @@
       </c>
       <c r="H79">
         <f t="shared" si="60"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -5144,7 +5145,7 @@
       </c>
       <c r="H80">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -5177,7 +5178,7 @@
       </c>
       <c r="H81">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -5210,7 +5211,7 @@
       </c>
       <c r="H82">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -5243,7 +5244,7 @@
       </c>
       <c r="H83">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -5309,7 +5310,7 @@
       </c>
       <c r="H85">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -5342,7 +5343,7 @@
       </c>
       <c r="H86">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
@@ -5375,7 +5376,7 @@
       </c>
       <c r="H87">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -5408,7 +5409,7 @@
       </c>
       <c r="H88">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -5474,7 +5475,7 @@
       </c>
       <c r="H90">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -5507,7 +5508,7 @@
       </c>
       <c r="H91">
         <f t="shared" si="60"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -5540,7 +5541,7 @@
       </c>
       <c r="H92">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
@@ -5573,7 +5574,7 @@
       </c>
       <c r="H93">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
@@ -5606,7 +5607,7 @@
       </c>
       <c r="H94">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
@@ -5639,7 +5640,7 @@
       </c>
       <c r="H95">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
@@ -5705,7 +5706,7 @@
       </c>
       <c r="H97">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -5738,7 +5739,7 @@
       </c>
       <c r="H98">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
@@ -5771,7 +5772,7 @@
       </c>
       <c r="H99">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
@@ -5804,7 +5805,7 @@
       </c>
       <c r="H100">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
@@ -5870,7 +5871,7 @@
       </c>
       <c r="H102">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
@@ -5903,7 +5904,7 @@
       </c>
       <c r="H103">
         <f t="shared" si="60"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
@@ -5936,7 +5937,7 @@
       </c>
       <c r="H104">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
@@ -5969,7 +5970,7 @@
       </c>
       <c r="H105">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
@@ -6002,7 +6003,7 @@
       </c>
       <c r="H106">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
@@ -6035,7 +6036,7 @@
       </c>
       <c r="H107">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
@@ -6101,7 +6102,7 @@
       </c>
       <c r="H109">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
@@ -6134,7 +6135,7 @@
       </c>
       <c r="H110">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
@@ -6167,7 +6168,7 @@
       </c>
       <c r="H111">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
@@ -6200,7 +6201,7 @@
       </c>
       <c r="H112">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
@@ -6266,7 +6267,7 @@
       </c>
       <c r="H114">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
@@ -6299,7 +6300,7 @@
       </c>
       <c r="H115">
         <f t="shared" si="60"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
@@ -6332,7 +6333,7 @@
       </c>
       <c r="H116">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
@@ -6365,7 +6366,7 @@
       </c>
       <c r="H117">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
@@ -6398,7 +6399,7 @@
       </c>
       <c r="H118">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
@@ -6431,7 +6432,7 @@
       </c>
       <c r="H119">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
@@ -6497,7 +6498,7 @@
       </c>
       <c r="H121">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
@@ -6530,7 +6531,7 @@
       </c>
       <c r="H122">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
@@ -6563,7 +6564,7 @@
       </c>
       <c r="H123">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
@@ -6596,7 +6597,7 @@
       </c>
       <c r="H124">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
@@ -6662,7 +6663,7 @@
       </c>
       <c r="H126">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
@@ -6695,7 +6696,7 @@
       </c>
       <c r="H127">
         <f t="shared" si="60"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
@@ -6728,7 +6729,7 @@
       </c>
       <c r="H128">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
@@ -6761,7 +6762,7 @@
       </c>
       <c r="H129">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
@@ -6794,7 +6795,7 @@
       </c>
       <c r="H130">
         <f t="shared" si="60"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -6827,7 +6828,7 @@
       </c>
       <c r="H131">
         <f t="shared" si="60"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
@@ -6859,7 +6860,7 @@
         <v>37104</v>
       </c>
       <c r="H132">
-        <f t="shared" ref="H132:H195" si="129">G132-G131</f>
+        <f t="shared" ref="H132:H195" si="129">G133-G132</f>
         <v>31</v>
       </c>
     </row>
@@ -6893,7 +6894,7 @@
       </c>
       <c r="H133">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
@@ -6926,7 +6927,7 @@
       </c>
       <c r="H134">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
@@ -6959,7 +6960,7 @@
       </c>
       <c r="H135">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
@@ -6992,7 +6993,7 @@
       </c>
       <c r="H136">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
@@ -7058,7 +7059,7 @@
       </c>
       <c r="H138">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
@@ -7091,7 +7092,7 @@
       </c>
       <c r="H139">
         <f t="shared" si="129"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
@@ -7124,7 +7125,7 @@
       </c>
       <c r="H140">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
@@ -7157,7 +7158,7 @@
       </c>
       <c r="H141">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
@@ -7190,7 +7191,7 @@
       </c>
       <c r="H142">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
@@ -7223,7 +7224,7 @@
       </c>
       <c r="H143">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
@@ -7289,7 +7290,7 @@
       </c>
       <c r="H145">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -7322,7 +7323,7 @@
       </c>
       <c r="H146">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -7355,7 +7356,7 @@
       </c>
       <c r="H147">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -7388,7 +7389,7 @@
       </c>
       <c r="H148">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -7454,7 +7455,7 @@
       </c>
       <c r="H150">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
@@ -7487,7 +7488,7 @@
       </c>
       <c r="H151">
         <f t="shared" si="129"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -7520,7 +7521,7 @@
       </c>
       <c r="H152">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -7553,7 +7554,7 @@
       </c>
       <c r="H153">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
@@ -7586,7 +7587,7 @@
       </c>
       <c r="H154">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
@@ -7619,7 +7620,7 @@
       </c>
       <c r="H155">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
@@ -7685,7 +7686,7 @@
       </c>
       <c r="H157">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -7718,7 +7719,7 @@
       </c>
       <c r="H158">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
@@ -7751,7 +7752,7 @@
       </c>
       <c r="H159">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -7784,7 +7785,7 @@
       </c>
       <c r="H160">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
@@ -7850,7 +7851,7 @@
       </c>
       <c r="H162">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
@@ -7883,7 +7884,7 @@
       </c>
       <c r="H163">
         <f t="shared" si="129"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
@@ -7916,7 +7917,7 @@
       </c>
       <c r="H164">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
@@ -7949,7 +7950,7 @@
       </c>
       <c r="H165">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
@@ -7982,7 +7983,7 @@
       </c>
       <c r="H166">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
@@ -8015,7 +8016,7 @@
       </c>
       <c r="H167">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
@@ -8081,7 +8082,7 @@
       </c>
       <c r="H169">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
@@ -8114,7 +8115,7 @@
       </c>
       <c r="H170">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
@@ -8147,7 +8148,7 @@
       </c>
       <c r="H171">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
@@ -8180,7 +8181,7 @@
       </c>
       <c r="H172">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
@@ -8246,7 +8247,7 @@
       </c>
       <c r="H174">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
@@ -8279,7 +8280,7 @@
       </c>
       <c r="H175">
         <f t="shared" si="129"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
@@ -8312,7 +8313,7 @@
       </c>
       <c r="H176">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
@@ -8345,7 +8346,7 @@
       </c>
       <c r="H177">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
@@ -8378,7 +8379,7 @@
       </c>
       <c r="H178">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
@@ -8411,7 +8412,7 @@
       </c>
       <c r="H179">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
@@ -8477,7 +8478,7 @@
       </c>
       <c r="H181">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
@@ -8510,7 +8511,7 @@
       </c>
       <c r="H182">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
@@ -8543,7 +8544,7 @@
       </c>
       <c r="H183">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
@@ -8576,7 +8577,7 @@
       </c>
       <c r="H184">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
@@ -8642,7 +8643,7 @@
       </c>
       <c r="H186">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
@@ -8675,7 +8676,7 @@
       </c>
       <c r="H187">
         <f t="shared" si="129"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
@@ -8708,7 +8709,7 @@
       </c>
       <c r="H188">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
@@ -8741,7 +8742,7 @@
       </c>
       <c r="H189">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
@@ -8774,7 +8775,7 @@
       </c>
       <c r="H190">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
@@ -8807,7 +8808,7 @@
       </c>
       <c r="H191">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
@@ -8873,7 +8874,7 @@
       </c>
       <c r="H193">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
@@ -8906,7 +8907,7 @@
       </c>
       <c r="H194">
         <f t="shared" si="129"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
@@ -8939,7 +8940,7 @@
       </c>
       <c r="H195">
         <f t="shared" si="129"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
@@ -8971,8 +8972,8 @@
         <v>39052</v>
       </c>
       <c r="H196">
-        <f t="shared" ref="H196:H259" si="200">G196-G195</f>
-        <v>30</v>
+        <f t="shared" ref="H196:H259" si="200">G197-G196</f>
+        <v>31</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
@@ -9038,7 +9039,7 @@
       </c>
       <c r="H198">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
@@ -9071,7 +9072,7 @@
       </c>
       <c r="H199">
         <f t="shared" si="200"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
@@ -9104,7 +9105,7 @@
       </c>
       <c r="H200">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
@@ -9137,7 +9138,7 @@
       </c>
       <c r="H201">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
@@ -9170,7 +9171,7 @@
       </c>
       <c r="H202">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
@@ -9203,7 +9204,7 @@
       </c>
       <c r="H203">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
@@ -9269,7 +9270,7 @@
       </c>
       <c r="H205">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
@@ -9302,7 +9303,7 @@
       </c>
       <c r="H206">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
@@ -9335,7 +9336,7 @@
       </c>
       <c r="H207">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
@@ -9368,7 +9369,7 @@
       </c>
       <c r="H208">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
@@ -9434,7 +9435,7 @@
       </c>
       <c r="H210">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
@@ -9467,7 +9468,7 @@
       </c>
       <c r="H211">
         <f t="shared" si="200"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
@@ -9500,7 +9501,7 @@
       </c>
       <c r="H212">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
@@ -9533,7 +9534,7 @@
       </c>
       <c r="H213">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
@@ -9566,7 +9567,7 @@
       </c>
       <c r="H214">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
@@ -9599,7 +9600,7 @@
       </c>
       <c r="H215">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
@@ -9665,7 +9666,7 @@
       </c>
       <c r="H217">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
@@ -9698,7 +9699,7 @@
       </c>
       <c r="H218">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
@@ -9731,7 +9732,7 @@
       </c>
       <c r="H219">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
@@ -9764,7 +9765,7 @@
       </c>
       <c r="H220">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
@@ -9830,7 +9831,7 @@
       </c>
       <c r="H222">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
@@ -9863,7 +9864,7 @@
       </c>
       <c r="H223">
         <f t="shared" si="200"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
@@ -9896,7 +9897,7 @@
       </c>
       <c r="H224">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
@@ -9929,7 +9930,7 @@
       </c>
       <c r="H225">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
@@ -9962,7 +9963,7 @@
       </c>
       <c r="H226">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
@@ -9995,7 +9996,7 @@
       </c>
       <c r="H227">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
@@ -10061,7 +10062,7 @@
       </c>
       <c r="H229">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
@@ -10094,7 +10095,7 @@
       </c>
       <c r="H230">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
@@ -10127,7 +10128,7 @@
       </c>
       <c r="H231">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
@@ -10160,7 +10161,7 @@
       </c>
       <c r="H232">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
@@ -10226,7 +10227,7 @@
       </c>
       <c r="H234">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
@@ -10259,7 +10260,7 @@
       </c>
       <c r="H235">
         <f t="shared" si="200"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
@@ -10292,7 +10293,7 @@
       </c>
       <c r="H236">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
@@ -10325,7 +10326,7 @@
       </c>
       <c r="H237">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
@@ -10358,7 +10359,7 @@
       </c>
       <c r="H238">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
@@ -10391,7 +10392,7 @@
       </c>
       <c r="H239">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
@@ -10457,7 +10458,7 @@
       </c>
       <c r="H241">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
@@ -10490,7 +10491,7 @@
       </c>
       <c r="H242">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -10523,7 +10524,7 @@
       </c>
       <c r="H243">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
@@ -10556,7 +10557,7 @@
       </c>
       <c r="H244">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
@@ -10622,7 +10623,7 @@
       </c>
       <c r="H246">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.3">
@@ -10655,7 +10656,7 @@
       </c>
       <c r="H247">
         <f t="shared" si="200"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.3">
@@ -10688,7 +10689,7 @@
       </c>
       <c r="H248">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.3">
@@ -10721,7 +10722,7 @@
       </c>
       <c r="H249">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.3">
@@ -10754,7 +10755,7 @@
       </c>
       <c r="H250">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.3">
@@ -10787,7 +10788,7 @@
       </c>
       <c r="H251">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.3">
@@ -10853,7 +10854,7 @@
       </c>
       <c r="H253">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.3">
@@ -10886,7 +10887,7 @@
       </c>
       <c r="H254">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.3">
@@ -10919,7 +10920,7 @@
       </c>
       <c r="H255">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.3">
@@ -10952,7 +10953,7 @@
       </c>
       <c r="H256">
         <f t="shared" si="200"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.3">
@@ -11018,7 +11019,7 @@
       </c>
       <c r="H258">
         <f t="shared" si="200"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.3">
@@ -11051,7 +11052,7 @@
       </c>
       <c r="H259">
         <f t="shared" si="200"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.3">
@@ -11083,8 +11084,8 @@
         <v>41000</v>
       </c>
       <c r="H260">
-        <f t="shared" ref="H260:H323" si="269">G260-G259</f>
-        <v>31</v>
+        <f t="shared" ref="H260:H323" si="269">G261-G260</f>
+        <v>30</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.3">
@@ -11117,7 +11118,7 @@
       </c>
       <c r="H261">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.3">
@@ -11150,7 +11151,7 @@
       </c>
       <c r="H262">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.3">
@@ -11183,7 +11184,7 @@
       </c>
       <c r="H263">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.3">
@@ -11249,7 +11250,7 @@
       </c>
       <c r="H265">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.3">
@@ -11282,7 +11283,7 @@
       </c>
       <c r="H266">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.3">
@@ -11315,7 +11316,7 @@
       </c>
       <c r="H267">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.3">
@@ -11348,7 +11349,7 @@
       </c>
       <c r="H268">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.3">
@@ -11414,7 +11415,7 @@
       </c>
       <c r="H270">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.3">
@@ -11447,7 +11448,7 @@
       </c>
       <c r="H271">
         <f t="shared" si="269"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.3">
@@ -11480,7 +11481,7 @@
       </c>
       <c r="H272">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.3">
@@ -11513,7 +11514,7 @@
       </c>
       <c r="H273">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.3">
@@ -11546,7 +11547,7 @@
       </c>
       <c r="H274">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.3">
@@ -11579,7 +11580,7 @@
       </c>
       <c r="H275">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.3">
@@ -11645,7 +11646,7 @@
       </c>
       <c r="H277">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.3">
@@ -11678,7 +11679,7 @@
       </c>
       <c r="H278">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.3">
@@ -11711,7 +11712,7 @@
       </c>
       <c r="H279">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.3">
@@ -11744,7 +11745,7 @@
       </c>
       <c r="H280">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.3">
@@ -11810,7 +11811,7 @@
       </c>
       <c r="H282">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.3">
@@ -11843,7 +11844,7 @@
       </c>
       <c r="H283">
         <f t="shared" si="269"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.3">
@@ -11876,7 +11877,7 @@
       </c>
       <c r="H284">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.3">
@@ -11909,7 +11910,7 @@
       </c>
       <c r="H285">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.3">
@@ -11942,7 +11943,7 @@
       </c>
       <c r="H286">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.3">
@@ -11975,7 +11976,7 @@
       </c>
       <c r="H287">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.3">
@@ -12041,7 +12042,7 @@
       </c>
       <c r="H289">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.3">
@@ -12074,7 +12075,7 @@
       </c>
       <c r="H290">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.3">
@@ -12107,7 +12108,7 @@
       </c>
       <c r="H291">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.3">
@@ -12140,7 +12141,7 @@
       </c>
       <c r="H292">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.3">
@@ -12206,7 +12207,7 @@
       </c>
       <c r="H294">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.3">
@@ -12239,7 +12240,7 @@
       </c>
       <c r="H295">
         <f t="shared" si="269"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.3">
@@ -12272,7 +12273,7 @@
       </c>
       <c r="H296">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.3">
@@ -12305,7 +12306,7 @@
       </c>
       <c r="H297">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.3">
@@ -12338,7 +12339,7 @@
       </c>
       <c r="H298">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.3">
@@ -12371,7 +12372,7 @@
       </c>
       <c r="H299">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.3">
@@ -12437,7 +12438,7 @@
       </c>
       <c r="H301">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.3">
@@ -12470,7 +12471,7 @@
       </c>
       <c r="H302">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.3">
@@ -12503,7 +12504,7 @@
       </c>
       <c r="H303">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.3">
@@ -12536,7 +12537,7 @@
       </c>
       <c r="H304">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.3">
@@ -12602,7 +12603,7 @@
       </c>
       <c r="H306">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.3">
@@ -12635,7 +12636,7 @@
       </c>
       <c r="H307">
         <f t="shared" si="269"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.3">
@@ -12668,7 +12669,7 @@
       </c>
       <c r="H308">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.3">
@@ -12701,7 +12702,7 @@
       </c>
       <c r="H309">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.3">
@@ -12734,7 +12735,7 @@
       </c>
       <c r="H310">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.3">
@@ -12767,7 +12768,7 @@
       </c>
       <c r="H311">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.3">
@@ -12833,7 +12834,7 @@
       </c>
       <c r="H313">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.3">
@@ -12866,7 +12867,7 @@
       </c>
       <c r="H314">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.3">
@@ -12899,7 +12900,7 @@
       </c>
       <c r="H315">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.3">
@@ -12932,7 +12933,7 @@
       </c>
       <c r="H316">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.3">
@@ -12998,7 +12999,7 @@
       </c>
       <c r="H318">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.3">
@@ -13031,7 +13032,7 @@
       </c>
       <c r="H319">
         <f t="shared" si="269"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.3">
@@ -13064,7 +13065,7 @@
       </c>
       <c r="H320">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.3">
@@ -13097,7 +13098,7 @@
       </c>
       <c r="H321">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.3">
@@ -13130,7 +13131,7 @@
       </c>
       <c r="H322">
         <f t="shared" si="269"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.3">
@@ -13163,7 +13164,7 @@
       </c>
       <c r="H323">
         <f t="shared" si="269"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.3">
@@ -13195,7 +13196,7 @@
         <v>42948</v>
       </c>
       <c r="H324">
-        <f t="shared" ref="H324:H337" si="340">G324-G323</f>
+        <f t="shared" ref="H324:H337" si="340">G325-G324</f>
         <v>31</v>
       </c>
     </row>
@@ -13229,7 +13230,7 @@
       </c>
       <c r="H325">
         <f t="shared" si="340"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.3">
@@ -13262,7 +13263,7 @@
       </c>
       <c r="H326">
         <f t="shared" si="340"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.3">
@@ -13295,7 +13296,7 @@
       </c>
       <c r="H327">
         <f t="shared" si="340"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.3">
@@ -13328,7 +13329,7 @@
       </c>
       <c r="H328">
         <f t="shared" si="340"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.3">
@@ -13394,7 +13395,7 @@
       </c>
       <c r="H330">
         <f t="shared" si="340"/>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.3">
@@ -13427,7 +13428,7 @@
       </c>
       <c r="H331">
         <f t="shared" si="340"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.3">
@@ -13460,7 +13461,7 @@
       </c>
       <c r="H332">
         <f t="shared" si="340"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.3">
@@ -13493,7 +13494,7 @@
       </c>
       <c r="H333">
         <f t="shared" si="340"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.3">
@@ -13526,7 +13527,7 @@
       </c>
       <c r="H334">
         <f t="shared" si="340"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.3">
@@ -13559,7 +13560,7 @@
       </c>
       <c r="H335">
         <f t="shared" si="340"/>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.3">
@@ -13623,9 +13624,14 @@
         <f t="shared" si="338"/>
         <v>43344</v>
       </c>
-      <c r="H337">
-        <f t="shared" si="340"/>
-        <v>31</v>
+      <c r="H337" s="7">
+        <f>G338-G337</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G338" s="32">
+        <v>43374</v>
       </c>
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
.hob update scripted. Outstanding to dos remain (listed in R file)
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907A6F57-74E4-40E0-BFCD-34E301B6774D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B37D2B-87EF-4B1A-9503-2BB3DFD1EC48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_file_dictionary" sheetId="5" r:id="rId1"/>
@@ -507,9 +507,6 @@
     <t>SVIHM.ets</t>
   </si>
   <si>
-    <t>getting there</t>
-  </si>
-  <si>
     <r>
       <t>Head observation file. Preamble, then, for each well, a row containing: location name, layer, row, column, number of stress periods containing an observation (listed as a negative number), an offset time from the start of the stress period (seems to be used for a structure where each location has one obselvation; it's just 0 for all of ours), row and column offset from center of cell (as fractions of cell width or height; all of ours are located in the middle of a quadrant, specified with + or - 0.25 offsets), and some extra parameters. For each observation under that well, list the unique observation identifier (built on the location name), the stress period in which the measurement was made, the number of time steps into the stress period, the head measurement (meters above mean sea level), and some extra parameters.</t>
     </r>
@@ -535,6 +532,9 @@
       <t>Make to do list in here</t>
     </r>
   </si>
+  <si>
+    <t>drafted with outstanding to dos</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +557,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +612,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -651,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -719,6 +725,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1799,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2322,12 +2331,12 @@
       <c r="B37" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>146</v>
+      <c r="C37" s="33" t="s">
+        <v>147</v>
       </c>
       <c r="D37" s="31"/>
       <c r="E37" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -2559,7 +2568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+    <sheetView topLeftCell="A311" workbookViewId="0">
       <selection activeCell="H337" sqref="H337"/>
     </sheetView>
   </sheetViews>
@@ -13196,7 +13205,7 @@
         <v>42948</v>
       </c>
       <c r="H324">
-        <f t="shared" ref="H324:H337" si="340">G325-G324</f>
+        <f t="shared" ref="H324:H336" si="340">G325-G324</f>
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
.oc file update scripted
</commit_message>
<xml_diff>
--- a/SWBM/update2018notes/notes.xlsx
+++ b/SWBM/update2018notes/notes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B37D2B-87EF-4B1A-9503-2BB3DFD1EC48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1787EBB0-AE69-4879-83D8-D5277F1BEF50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="150">
   <si>
     <t>year</t>
   </si>
@@ -534,6 +534,12 @@
   </si>
   <si>
     <t>drafted with outstanding to dos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lists all the output file types and names (e.g., hob for head observations). </t>
+  </si>
+  <si>
+    <t>Controls when the water budget is saved (after every stress period)</t>
   </si>
 </sst>
 </file>
@@ -1808,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586B933-D340-49CB-AB4A-230CE00A6B42}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2346,11 +2352,13 @@
       <c r="B38" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>114</v>
+      <c r="C38" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D38" s="16"/>
-      <c r="E38" s="30"/>
+      <c r="E38" s="30" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
@@ -2359,8 +2367,8 @@
       <c r="B39" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>114</v>
+      <c r="C39" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="30"/>
@@ -2372,11 +2380,13 @@
       <c r="B40" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>114</v>
+      <c r="C40" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="D40" s="16"/>
-      <c r="E40" s="30"/>
+      <c r="E40" s="30" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">

</xml_diff>